<commit_message>
add all files and restructure methods
</commit_message>
<xml_diff>
--- a/Elements/Datas/Stats/clustercenters.xlsx
+++ b/Elements/Datas/Stats/clustercenters.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,53 +462,87 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>17</v>
+        <v>13.9064</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.2606</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1.926</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1.9842</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.3761</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>9</v>
+        <v>21.8247</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>0.3299</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>1.9468</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.9789</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.1746</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>24</v>
+        <v>6.2136</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.1743</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1.3003</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>3.8979</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.6026</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>17.5509</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5616</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6.3853</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.4442</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>8.047599999999999</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1201</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5.8881</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.6037</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.4569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>